<commit_message>
wokrblocks now only pass path to children wbs
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mihai.dunareanu\Google Drive\Workspace\UiPath\Templates\UiPEngineLocalProcess\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mihai.dunareanu\Documents\UiPath\UiPEngineLocalProcess\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAEB3021-EB07-4562-A3E5-FD501D3942F5}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D516345-F34F-4BDC-B9A9-8850DE1634CD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="7" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -164,9 +164,6 @@
     <t>UiDemoPath</t>
   </si>
   <si>
-    <t>Resources\uidemo_login\UiDemo.exe</t>
-  </si>
-  <si>
     <t>UiPath application path</t>
   </si>
   <si>
@@ -177,6 +174,12 @@
   </si>
   <si>
     <t>This key belongs to user designated category 2</t>
+  </si>
+  <si>
+    <t>C:\Users\mihai.dunareanu\Documents\UiPath\UiPEngineLocalProcess\Resources\uidemo_login\UiDemo.exe</t>
+  </si>
+  <si>
+    <t>UiDemoCredential</t>
   </si>
 </sst>
 </file>
@@ -686,7 +689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{358C8B53-A61E-4F05-B727-D34F2E27D989}">
   <dimension ref="A1:A18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -778,7 +781,7 @@
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -792,7 +795,7 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -853,21 +856,21 @@
         <v>45</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
         <v>46</v>
-      </c>
-      <c r="C3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="3">
         <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" ht="14.25" customHeight="1"/>
@@ -1853,8 +1856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EBC672C-F735-4EF3-8287-9B35E6A7A36A}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1898,6 +1901,14 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
+    </row>
+    <row r="2" spans="1:26" ht="15" customHeight="1">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
@@ -2874,6 +2885,7 @@
     <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>